<commit_message>
pricing for 2nd computer
</commit_message>
<xml_diff>
--- a/guides/Computer Parts 2020_11_22.xlsx
+++ b/guides/Computer Parts 2020_11_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\notes\guides\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A0A1133-16E8-4B8D-948D-C6D91D879FC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AE8579DE-E774-480F-B6B3-48B41C6EC8AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32340" yWindow="2130" windowWidth="21600" windowHeight="11385" xr2:uid="{19E93823-BD21-4BBC-A3DA-4F1CCE8F76E1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{19E93823-BD21-4BBC-A3DA-4F1CCE8F76E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>CPU</t>
   </si>
@@ -87,9 +87,6 @@
     <t>G-SKILL 64 GB ddr4 3200</t>
   </si>
   <si>
-    <t>https://www.newegg.com/g-skill-64gb-288-pin-ddr4-sdram/p/N82E16820232092?Item=N82E16820232092</t>
-  </si>
-  <si>
     <t>https://www.newegg.com/samsung-970-evo-plus-2tb/p/N82E16820147744</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>https://www.newegg.com/asus-geforce-rtx-2060-dual-rtx2060-o6g-evo/p/N82E16814126349?Item=N82E16814126349</t>
-  </si>
-  <si>
     <t>https://www.newegg.com/thermaltake-toughpower-gf1-tt-premium-edition-ps-tpd-0850fnfaga-1-850w/p/N82E16817153403</t>
   </si>
   <si>
@@ -109,24 +103,58 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Intel Core i17 9700K</t>
+  </si>
+  <si>
+    <t>https://www.newegg.com/core-i7-9th-gen-intel-core-i7-9700k/p/N82E16819117958</t>
+  </si>
+  <si>
+    <t>G-SKILL 32 GB ddr4 3200</t>
+  </si>
+  <si>
+    <t>https://www.newegg.com/samsung-970-evo-plus-1tb/p/N82E16820147743</t>
+  </si>
+  <si>
+    <t>https://www.newegg.com/msi-geforce-gtx-1650-gtx-1650-d6-gaming-x/p/N82E16814137527</t>
+  </si>
+  <si>
+    <t>1TB Samsung 970 evo plus NVMe SSD</t>
+  </si>
+  <si>
+    <t>Asus Geforce GTX 1650 dual-fan</t>
+  </si>
+  <si>
+    <t>https://www.newegg.com/g-skill-32gb-288-pin-ddr4-sdram/p/N82E16820232886</t>
+  </si>
+  <si>
+    <t>Thermaltake 650W modular</t>
+  </si>
+  <si>
+    <t>https://www.newegg.com/thermaltake-toughpower-gf1-tt-premium-edition-ps-tpd-0650fnfaga-1-650w/p/N82E16817153396</t>
+  </si>
+  <si>
+    <t>https://www.newegg.com/g-skill-64gb-288-pin-ddr4-sdram/p/N82E16820232092</t>
+  </si>
+  <si>
+    <t>https://www.newegg.com/asus-geforce-rtx-2060-dual-rtx2060-o6g-evo/p/N82E16814126349</t>
+  </si>
+  <si>
+    <t>https://www.newegg.com/cooler-master-masterliquid-ml240l-rgb-liquid-cooling-system/p/2YM-0004-00015</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
     <font>
       <sz val="11"/>
@@ -139,13 +167,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,17 +191,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -498,17 +516,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B93FA1-FCEE-4753-95C9-56CF7AF7A4E5}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.140625" customWidth="1"/>
     <col min="2" max="2" width="72.42578125" customWidth="1"/>
-    <col min="4" max="4" width="90.42578125" customWidth="1"/>
+    <col min="4" max="4" width="142.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -524,9 +542,9 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>475</v>
-      </c>
-      <c r="D2" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -534,13 +552,13 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C3">
-        <v>180</v>
-      </c>
-      <c r="D3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -552,10 +570,10 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <v>220</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>17</v>
+        <v>210</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -568,8 +586,8 @@
       <c r="C5">
         <v>249</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -579,8 +597,8 @@
       <c r="C6">
         <v>249</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
+      <c r="D6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -588,13 +606,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7">
         <v>330</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
+      <c r="D7" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -602,7 +620,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8">
         <v>100</v>
@@ -612,14 +630,14 @@
       <c r="A9" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C9">
-        <v>75</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>60</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,17 +650,135 @@
       <c r="C10">
         <v>130</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11">
         <f>SUM(C2:C10)</f>
-        <v>2008</v>
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>260</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>190</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16">
+        <v>120</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>150</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18">
+        <v>188</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21">
+        <v>70</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <f>SUM(C14:C21)</f>
+        <v>1138</v>
       </c>
     </row>
   </sheetData>
@@ -650,8 +786,20 @@
     <hyperlink ref="D6" r:id="rId1" xr:uid="{FA506B96-06CE-4CD1-8D0C-30C27B59EE3A}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{33B7CED8-CE81-40D9-AF7A-2962E2BD4822}"/>
     <hyperlink ref="D10" r:id="rId3" xr:uid="{386C8F6A-9EB2-4F5F-89CD-2F09FABAA210}"/>
+    <hyperlink ref="D18" r:id="rId4" xr:uid="{25865888-FE7A-4BB4-AE05-B38B8F8B2318}"/>
+    <hyperlink ref="D14" r:id="rId5" xr:uid="{D2B472C5-92B4-407F-85AA-2F684B414F0A}"/>
+    <hyperlink ref="D15" r:id="rId6" xr:uid="{DCA82397-9A77-4ED1-9403-18D104360FAE}"/>
+    <hyperlink ref="D16" r:id="rId7" xr:uid="{DD7517F5-0BD4-4A3B-B558-F715C2406E5A}"/>
+    <hyperlink ref="D17" r:id="rId8" xr:uid="{129896A5-CC54-478D-8579-D3AD5B0918A6}"/>
+    <hyperlink ref="D21" r:id="rId9" xr:uid="{887E6612-8C3C-4444-A982-6ED57E29CDC3}"/>
+    <hyperlink ref="D20" r:id="rId10" xr:uid="{AB441EF8-6614-4D8A-987A-0B37BDC1398C}"/>
+    <hyperlink ref="D2" r:id="rId11" xr:uid="{AE6DFB91-448B-4641-B6CE-1E1FDD2F4850}"/>
+    <hyperlink ref="D3" r:id="rId12" xr:uid="{E2BCF434-739B-4869-8773-145A93D490AA}"/>
+    <hyperlink ref="D4" r:id="rId13" xr:uid="{1107213B-BBCC-4614-8E70-2BDB8454D48B}"/>
+    <hyperlink ref="D7" r:id="rId14" xr:uid="{B99ED4F1-5B1C-4D35-A758-D06F22A33693}"/>
+    <hyperlink ref="D9" r:id="rId15" xr:uid="{3BE4AD33-4D89-41BD-876E-40F3FCEAFF38}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>